<commit_message>
string field must embrace with quote
</commit_message>
<xml_diff>
--- a/config/Template-模板.xlsx
+++ b/config/Template-模板.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21030" windowHeight="10890" tabRatio="841" activeTab="1"/>
+    <workbookView windowWidth="20355" windowHeight="10890" tabRatio="841"/>
   </bookViews>
   <sheets>
     <sheet name="tiny-tpl" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
     <t>example_key</t>
   </si>
   <si>
-    <t>example_value</t>
+    <t>"example value"</t>
   </si>
   <si>
     <t>演示字段备注</t>
@@ -98,7 +98,7 @@
     <t>每一行是一条记录</t>
   </si>
   <si>
-    <t>test_name</t>
+    <t>"test_name"</t>
   </si>
 </sst>
 </file>
@@ -159,53 +159,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,43 +172,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="华文中宋"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="华文细黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -266,21 +188,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="华文细黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF3F3F76"/>
-      <name val="华文细黑"/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="华文中宋"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,16 +230,72 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="新宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="华文新魏"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="0"/>
       <name val="新宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="5" tint="-0.249977111117893"/>
-      <name val="华文新魏"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -323,19 +306,32 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="华文细黑"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -345,6 +341,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="12"/>
       <color theme="9" tint="-0.249946592608417"/>
@@ -352,21 +364,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="新宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFC00000"/>
       <name val="华文中宋"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -439,19 +439,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,19 +457,71 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="0" tint="-0.0499893185216834"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="0" tint="-0.149906918546098"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="9" tint="0.599993896298105"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,19 +533,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,91 +545,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0499893185216834"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,19 +567,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,24 +627,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
-      <gradientFill degree="90">
-        <stop position="0">
-          <color theme="0"/>
-        </stop>
-        <stop position="1">
-          <color theme="9" tint="0.599993896298105"/>
-        </stop>
-      </gradientFill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149906918546098"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -749,21 +749,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -778,29 +763,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -820,6 +793,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -831,16 +819,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -859,17 +843,33 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -879,204 +879,204 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="11" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="6" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="9" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="40" borderId="6">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="13" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="14" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="41" borderId="11" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="9" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="6" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="9" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="6" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="39" borderId="9" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="42" borderId="0" applyAlignment="0">
@@ -1087,7 +1087,7 @@
     </xf>
     <xf numFmtId="0" fontId="40" fillId="44" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1124,9 +1124,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1220,8 +1217,8 @@
     <cellStyle name="我的单元格1" xfId="59"/>
     <cellStyle name="我的单元格3" xfId="60"/>
     <cellStyle name="我的单元格4" xfId="61"/>
-    <cellStyle name="我的外边框" xfId="62"/>
-    <cellStyle name="我的公式2" xfId="63"/>
+    <cellStyle name="我的公式2" xfId="62"/>
+    <cellStyle name="我的外边框" xfId="63"/>
     <cellStyle name="我的链接" xfId="64"/>
     <cellStyle name="我的英文1" xfId="65"/>
     <cellStyle name="我的英文2" xfId="66"/>
@@ -1240,7 +1237,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{54511284-822a-4f3f-af7b-8a0040c7d409}" diskRevisions="1" revisionId="16" version="10">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8f210f53-450b-4a38-9139-2ddcd3db5f9a}" diskRevisions="1" revisionId="20" version="14">
   <header guid="{00cd06d3-a7dd-4d37-ad9c-2428ecb2d1e1}" dateTime="2020-02-22T11:35:33" maxSheetId="3" userName="willz" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1296,6 +1293,30 @@
     </sheetIdMap>
   </header>
   <header guid="{54511284-822a-4f3f-af7b-8a0040c7d409}" dateTime="2020-02-22T11:45:07" maxSheetId="3" userName="willz" r:id="rId10" minRId="10" maxRId="16">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{d503539e-32e4-4bca-8041-10808b91f215}" dateTime="2020-02-22T11:47:44" maxSheetId="3" userName="willz" r:id="rId11" minRId="17">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{c00863b4-cccb-4d85-a8fa-c279a85070d5}" dateTime="2020-02-22T11:47:51" maxSheetId="3" userName="willz" r:id="rId12" minRId="18">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{a04b2295-cb7d-4952-bee9-8e8defc8bb30}" dateTime="2020-02-22T11:48:25" maxSheetId="3" userName="willz" r:id="rId13" minRId="19">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8f210f53-450b-4a38-9139-2ddcd3db5f9a}" dateTime="2020-02-22T11:48:34" maxSheetId="3" userName="willz" r:id="rId14" minRId="20">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1365,6 +1386,74 @@
   <rcc rId="16" sId="2">
     <nc r="B8" t="n">
       <v>100</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="17" sId="2">
+    <oc r="C8" t="inlineStr">
+      <is>
+        <t>test_name</t>
+      </is>
+    </oc>
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>"test_name"</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="18" sId="1">
+    <oc r="D6" t="inlineStr">
+      <is>
+        <t>example_value</t>
+      </is>
+    </oc>
+    <nc r="D6" t="inlineStr">
+      <is>
+        <t>"example_value"</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="19" sId="1">
+    <oc r="D6" t="inlineStr">
+      <is>
+        <t>"example_value"</t>
+      </is>
+    </oc>
+    <nc r="D6" t="inlineStr">
+      <is>
+        <t>example value</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="20" sId="1">
+    <oc r="D6" t="inlineStr">
+      <is>
+        <t>example value</t>
+      </is>
+    </oc>
+    <nc r="D6" t="inlineStr">
+      <is>
+        <t>"example value"</t>
+      </is>
     </nc>
   </rcc>
 </revisions>
@@ -1490,7 +1579,7 @@
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{54511284-822a-4f3f-af7b-8a0040c7d409}" name="willz" id="-878984565" dateTime="2020-02-22T11:40:48"/>
+  <userInfo guid="{8f210f53-450b-4a38-9139-2ddcd3db5f9a}" name="willz" id="-878991637" dateTime="2020-02-22T11:46:41"/>
 </users>
 </file>
 
@@ -1752,18 +1841,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E197"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="24.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="14" customWidth="1"/>
-    <col min="4" max="4" width="16.25" style="14" customWidth="1"/>
+    <col min="3" max="3" width="14.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
@@ -1772,13 +1861,13 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
@@ -1792,11 +1881,11 @@
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1804,22 +1893,22 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <v>0</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="19"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="9"/>
     </row>
     <row r="4" customFormat="1" spans="1:5">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="20"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1831,7 +1920,7 @@
       <c r="D5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1852,197 +1941,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1"/>
-    <row r="8" s="1" customFormat="1"/>
-    <row r="9" s="1" customFormat="1"/>
-    <row r="10" s="1" customFormat="1"/>
-    <row r="11" s="1" customFormat="1"/>
-    <row r="12" s="1" customFormat="1"/>
-    <row r="13" s="1" customFormat="1"/>
-    <row r="14" s="1" customFormat="1"/>
-    <row r="15" s="1" customFormat="1"/>
-    <row r="16" s="1" customFormat="1"/>
-    <row r="17" s="1" customFormat="1"/>
-    <row r="18" s="1" customFormat="1"/>
-    <row r="19" s="1" customFormat="1"/>
-    <row r="20" s="1" customFormat="1"/>
-    <row r="21" s="1" customFormat="1"/>
-    <row r="22" s="1" customFormat="1"/>
-    <row r="23" s="1" customFormat="1"/>
-    <row r="24" s="1" customFormat="1"/>
-    <row r="25" s="1" customFormat="1"/>
-    <row r="26" s="1" customFormat="1"/>
-    <row r="27" s="1" customFormat="1"/>
-    <row r="28" s="1" customFormat="1"/>
-    <row r="29" s="1" customFormat="1"/>
-    <row r="30" s="1" customFormat="1"/>
-    <row r="31" s="1" customFormat="1"/>
-    <row r="32" s="1" customFormat="1"/>
-    <row r="33" s="1" customFormat="1"/>
-    <row r="34" s="1" customFormat="1"/>
-    <row r="35" s="1" customFormat="1"/>
-    <row r="36" s="1" customFormat="1"/>
-    <row r="37" s="1" customFormat="1"/>
-    <row r="38" s="1" customFormat="1"/>
-    <row r="39" s="1" customFormat="1"/>
-    <row r="40" s="1" customFormat="1"/>
-    <row r="41" s="1" customFormat="1"/>
-    <row r="42" s="1" customFormat="1"/>
-    <row r="43" s="1" customFormat="1"/>
-    <row r="44" s="1" customFormat="1"/>
-    <row r="45" s="1" customFormat="1"/>
-    <row r="46" s="1" customFormat="1"/>
-    <row r="47" s="1" customFormat="1"/>
-    <row r="48" s="1" customFormat="1"/>
-    <row r="49" s="1" customFormat="1"/>
-    <row r="50" s="1" customFormat="1"/>
-    <row r="51" s="1" customFormat="1"/>
-    <row r="52" s="1" customFormat="1"/>
-    <row r="53" s="1" customFormat="1"/>
-    <row r="54" s="1" customFormat="1"/>
-    <row r="55" s="1" customFormat="1"/>
-    <row r="56" s="1" customFormat="1"/>
-    <row r="57" s="1" customFormat="1"/>
-    <row r="58" s="1" customFormat="1"/>
-    <row r="59" s="1" customFormat="1"/>
-    <row r="60" s="1" customFormat="1"/>
-    <row r="61" s="1" customFormat="1"/>
-    <row r="62" s="1" customFormat="1"/>
-    <row r="63" s="1" customFormat="1"/>
-    <row r="64" s="1" customFormat="1"/>
-    <row r="65" s="1" customFormat="1"/>
-    <row r="66" s="1" customFormat="1"/>
-    <row r="67" s="1" customFormat="1"/>
-    <row r="68" s="1" customFormat="1"/>
-    <row r="69" s="1" customFormat="1"/>
-    <row r="70" s="1" customFormat="1"/>
-    <row r="71" s="1" customFormat="1"/>
-    <row r="72" s="1" customFormat="1"/>
-    <row r="73" s="1" customFormat="1"/>
-    <row r="74" s="1" customFormat="1"/>
-    <row r="75" s="1" customFormat="1"/>
-    <row r="76" s="1" customFormat="1"/>
-    <row r="77" s="1" customFormat="1"/>
-    <row r="78" s="1" customFormat="1"/>
-    <row r="79" s="1" customFormat="1"/>
-    <row r="80" s="1" customFormat="1"/>
-    <row r="81" s="1" customFormat="1"/>
-    <row r="82" s="1" customFormat="1"/>
-    <row r="83" s="1" customFormat="1"/>
-    <row r="84" s="1" customFormat="1"/>
-    <row r="85" s="1" customFormat="1"/>
-    <row r="86" s="1" customFormat="1"/>
-    <row r="87" s="1" customFormat="1"/>
-    <row r="88" s="1" customFormat="1"/>
-    <row r="89" s="1" customFormat="1"/>
-    <row r="90" s="1" customFormat="1"/>
-    <row r="91" s="1" customFormat="1"/>
-    <row r="92" s="1" customFormat="1"/>
-    <row r="93" s="1" customFormat="1"/>
-    <row r="94" s="1" customFormat="1"/>
-    <row r="95" s="1" customFormat="1"/>
-    <row r="96" s="1" customFormat="1"/>
-    <row r="97" s="1" customFormat="1"/>
-    <row r="98" s="1" customFormat="1"/>
-    <row r="99" s="1" customFormat="1"/>
-    <row r="100" s="1" customFormat="1"/>
-    <row r="101" s="1" customFormat="1"/>
-    <row r="102" s="1" customFormat="1"/>
-    <row r="103" s="1" customFormat="1"/>
-    <row r="104" s="1" customFormat="1"/>
-    <row r="105" s="1" customFormat="1"/>
-    <row r="106" s="1" customFormat="1"/>
-    <row r="107" s="1" customFormat="1"/>
-    <row r="108" s="1" customFormat="1"/>
-    <row r="109" s="1" customFormat="1"/>
-    <row r="110" s="1" customFormat="1"/>
-    <row r="111" s="1" customFormat="1"/>
-    <row r="112" s="1" customFormat="1"/>
-    <row r="113" s="1" customFormat="1"/>
-    <row r="114" s="1" customFormat="1"/>
-    <row r="115" s="1" customFormat="1"/>
-    <row r="116" s="1" customFormat="1"/>
-    <row r="117" s="1" customFormat="1"/>
-    <row r="118" s="1" customFormat="1"/>
-    <row r="119" s="1" customFormat="1"/>
-    <row r="120" s="1" customFormat="1"/>
-    <row r="121" s="1" customFormat="1"/>
-    <row r="122" s="1" customFormat="1"/>
-    <row r="123" s="1" customFormat="1"/>
-    <row r="124" s="1" customFormat="1"/>
-    <row r="125" s="1" customFormat="1"/>
-    <row r="126" s="1" customFormat="1"/>
-    <row r="127" s="1" customFormat="1"/>
-    <row r="128" s="1" customFormat="1"/>
-    <row r="129" s="1" customFormat="1"/>
-    <row r="130" s="1" customFormat="1"/>
-    <row r="131" s="1" customFormat="1"/>
-    <row r="132" s="1" customFormat="1"/>
-    <row r="133" s="1" customFormat="1"/>
-    <row r="134" s="1" customFormat="1"/>
-    <row r="135" s="1" customFormat="1"/>
-    <row r="136" s="1" customFormat="1"/>
-    <row r="137" s="1" customFormat="1"/>
-    <row r="138" s="1" customFormat="1"/>
-    <row r="139" s="1" customFormat="1"/>
-    <row r="140" s="1" customFormat="1"/>
-    <row r="141" s="1" customFormat="1"/>
-    <row r="142" s="1" customFormat="1"/>
-    <row r="143" s="1" customFormat="1"/>
-    <row r="144" s="1" customFormat="1"/>
-    <row r="145" s="1" customFormat="1"/>
-    <row r="146" s="1" customFormat="1"/>
-    <row r="147" s="1" customFormat="1"/>
-    <row r="148" s="1" customFormat="1"/>
-    <row r="149" s="1" customFormat="1"/>
-    <row r="150" s="1" customFormat="1"/>
-    <row r="151" s="1" customFormat="1"/>
-    <row r="152" s="1" customFormat="1"/>
-    <row r="153" s="1" customFormat="1"/>
-    <row r="154" s="1" customFormat="1"/>
-    <row r="155" s="1" customFormat="1"/>
-    <row r="156" s="1" customFormat="1"/>
-    <row r="157" s="1" customFormat="1"/>
-    <row r="158" s="1" customFormat="1"/>
-    <row r="159" s="1" customFormat="1"/>
-    <row r="160" s="1" customFormat="1"/>
-    <row r="161" s="1" customFormat="1"/>
-    <row r="162" s="1" customFormat="1"/>
-    <row r="163" s="1" customFormat="1"/>
-    <row r="164" s="1" customFormat="1"/>
-    <row r="165" s="1" customFormat="1"/>
-    <row r="166" s="1" customFormat="1"/>
-    <row r="167" s="1" customFormat="1"/>
-    <row r="168" s="1" customFormat="1"/>
-    <row r="169" s="1" customFormat="1"/>
-    <row r="170" s="1" customFormat="1"/>
-    <row r="171" s="1" customFormat="1"/>
-    <row r="172" s="1" customFormat="1"/>
-    <row r="173" s="1" customFormat="1"/>
-    <row r="174" s="1" customFormat="1"/>
-    <row r="175" s="1" customFormat="1"/>
-    <row r="176" s="1" customFormat="1"/>
-    <row r="177" s="1" customFormat="1"/>
-    <row r="178" s="1" customFormat="1"/>
-    <row r="179" s="1" customFormat="1"/>
-    <row r="180" s="1" customFormat="1"/>
-    <row r="181" s="1" customFormat="1"/>
-    <row r="182" s="1" customFormat="1"/>
-    <row r="183" s="1" customFormat="1"/>
-    <row r="184" s="1" customFormat="1"/>
-    <row r="185" s="1" customFormat="1"/>
-    <row r="186" s="1" customFormat="1"/>
-    <row r="187" s="1" customFormat="1"/>
-    <row r="188" s="1" customFormat="1"/>
-    <row r="189" s="1" customFormat="1"/>
-    <row r="190" s="1" customFormat="1"/>
-    <row r="191" s="1" customFormat="1"/>
-    <row r="192" s="1" customFormat="1"/>
-    <row r="193" s="1" customFormat="1"/>
-    <row r="194" s="1" customFormat="1"/>
-    <row r="195" s="1" customFormat="1"/>
-    <row r="196" s="1" customFormat="1"/>
-    <row r="197" s="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2055,10 +1953,10 @@
   <sheetPr/>
   <dimension ref="A1:XFD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2280" topLeftCell="A1" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7"/>

</xml_diff>

<commit_message>
fix that string was converted to array
</commit_message>
<xml_diff>
--- a/config/Template-模板.xlsx
+++ b/config/Template-模板.xlsx
@@ -71,7 +71,7 @@
     <t>example_key</t>
   </si>
   <si>
-    <t>"example value"</t>
+    <t>"test example value"</t>
   </si>
   <si>
     <t>演示字段备注</t>
@@ -1087,7 +1087,7 @@
     </xf>
     <xf numFmtId="0" fontId="40" fillId="44" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1124,6 +1124,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1237,7 +1240,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8f210f53-450b-4a38-9139-2ddcd3db5f9a}" diskRevisions="1" revisionId="20" version="14">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{138d06bf-6eaf-419b-b109-ca2b670fa78c}" diskRevisions="1" revisionId="21" version="16">
   <header guid="{00cd06d3-a7dd-4d37-ad9c-2428ecb2d1e1}" dateTime="2020-02-22T11:35:33" maxSheetId="3" userName="willz" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1317,6 +1320,18 @@
     </sheetIdMap>
   </header>
   <header guid="{8f210f53-450b-4a38-9139-2ddcd3db5f9a}" dateTime="2020-02-22T11:48:34" maxSheetId="3" userName="willz" r:id="rId14" minRId="20">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{a64e1b06-03ba-4162-925a-ed916f353e02}" dateTime="2020-02-22T11:55:30" maxSheetId="3" userName="willz" r:id="rId15">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{138d06bf-6eaf-419b-b109-ca2b670fa78c}" dateTime="2020-02-22T11:56:19" maxSheetId="3" userName="willz" r:id="rId16" minRId="21">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1459,6 +1474,33 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="$A6:$XFD1048576" start="0" length="2147483647">
+    <dxf>
+      <numFmt numFmtId="49" formatCode="@"/>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="21" sId="1" numFmtId="30">
+    <oc r="D6" t="inlineStr">
+      <is>
+        <t>"example value"</t>
+      </is>
+    </oc>
+    <nc r="D6" t="inlineStr">
+      <is>
+        <t>"test example value"</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="1" sId="1">
@@ -1579,7 +1621,7 @@
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{8f210f53-450b-4a38-9139-2ddcd3db5f9a}" name="willz" id="-878991637" dateTime="2020-02-22T11:46:41"/>
+  <userInfo guid="{138d06bf-6eaf-419b-b109-ca2b670fa78c}" name="willz" id="-878991637" dateTime="2020-02-22T11:46:41"/>
 </users>
 </file>
 
@@ -1844,30 +1886,30 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="24.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="24.25" style="14" customWidth="1"/>
+    <col min="2" max="2" width="17.625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="14.25" style="14" customWidth="1"/>
+    <col min="4" max="4" width="16.25" style="14" customWidth="1"/>
+    <col min="5" max="5" width="26.625" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
@@ -1881,11 +1923,11 @@
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1893,22 +1935,22 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="16">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="18"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="9"/>
     </row>
     <row r="4" customFormat="1" spans="1:5">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="19"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20"/>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="21" t="s">
+    <row r="5" s="1" customFormat="1" spans="1:5">
+      <c r="A5" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1920,24 +1962,24 @@
       <c r="D5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:5">
-      <c r="A6" s="1" t="s">
+    <row r="6" s="14" customFormat="1" spans="1:5">
+      <c r="A6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1954,7 +1996,7 @@
   <dimension ref="A1:XFD8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2280" topLeftCell="A1" activePane="bottomLeft"/>
+      <pane ySplit="2280" topLeftCell="A4" activePane="bottomLeft"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>

</xml_diff>